<commit_message>
Human complaint classification in progress
</commit_message>
<xml_diff>
--- a/data/raw/01-06_human_feedback.xlsx
+++ b/data/raw/01-06_human_feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/foulds/code/dsm050-2023-apr/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFC40B2-C228-114F-B012-EF0B11B4DBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6187FDEF-F5CD-5746-82E1-389585B35C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="38380" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2833" uniqueCount="1847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2921" uniqueCount="1867">
   <si>
     <t>id</t>
   </si>
@@ -5896,10 +5896,70 @@
     <t>safety concern</t>
   </si>
   <si>
-    <t>new_complaint_classification</t>
-  </si>
-  <si>
-    <t>new_chatbot_classification</t>
+    <t>human_chatbot_classification</t>
+  </si>
+  <si>
+    <t>human_complaint_classification</t>
+  </si>
+  <si>
+    <t>blacklist</t>
+  </si>
+  <si>
+    <t>voice bundle</t>
+  </si>
+  <si>
+    <t>billing</t>
+  </si>
+  <si>
+    <t>data bundle</t>
+  </si>
+  <si>
+    <t>upgrade</t>
+  </si>
+  <si>
+    <t>fraud</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>new contract</t>
+  </si>
+  <si>
+    <t>subscription services</t>
+  </si>
+  <si>
+    <t>courier delivery</t>
+  </si>
+  <si>
+    <t>number does not exist</t>
+  </si>
+  <si>
+    <t>missing airtime</t>
+  </si>
+  <si>
+    <t>cancel bundle</t>
+  </si>
+  <si>
+    <t>downgrade account</t>
+  </si>
+  <si>
+    <t>vodamail</t>
+  </si>
+  <si>
+    <t>rewards</t>
+  </si>
+  <si>
+    <t>sim swap</t>
+  </si>
+  <si>
+    <t>vodabucks</t>
+  </si>
+  <si>
+    <t>sms spam</t>
   </si>
 </sst>
 </file>
@@ -6002,10 +6062,10 @@
     <tableColumn id="7" xr3:uid="{D9ED5856-D5F7-7A48-A394-8C39D6F1846C}" name="chatbot_related"/>
     <tableColumn id="8" xr3:uid="{2EA6229D-1C42-C343-A871-6D50576A407F}" name="chatbot_evidence"/>
     <tableColumn id="9" xr3:uid="{E438B2BC-6356-C244-AA96-AEC9F487FD90}" name="chatbot_classification" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{E0510D99-9D9F-8D4E-91AE-75B15AE48181}" name="new_chatbot_classification" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{E0510D99-9D9F-8D4E-91AE-75B15AE48181}" name="human_chatbot_classification" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{33648AB4-0FF8-B744-A440-19D06366560F}" name="chatbot_description" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{CF474B90-D10E-A845-AA71-0B8828A6FB7E}" name="chatbot_suggestion"/>
-    <tableColumn id="17" xr3:uid="{373162CA-6CF7-E245-80C7-4E322DA79A00}" name="new_complaint_classification"/>
+    <tableColumn id="17" xr3:uid="{373162CA-6CF7-E245-80C7-4E322DA79A00}" name="human_complaint_classification"/>
     <tableColumn id="12" xr3:uid="{E2DA2FE3-C658-954E-B672-53CA8896E68D}" name="complaint_classification" dataDxfId="2"/>
     <tableColumn id="13" xr3:uid="{203A7C9D-0399-A146-B8EE-46CD14D19095}" name="complaint_service" dataDxfId="1"/>
     <tableColumn id="14" xr3:uid="{DC475008-088B-7447-9799-7F1697516031}" name="complaint_description"/>
@@ -6302,8 +6362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J237" sqref="J237"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6315,11 +6375,10 @@
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="16" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="20.5" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="2" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
     <col min="14" max="14" width="22" style="2" customWidth="1"/>
     <col min="15" max="15" width="17.6640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="21" hidden="1" customWidth="1"/>
@@ -6355,7 +6414,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>9</v>
@@ -6364,7 +6423,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>11</v>
@@ -6416,6 +6475,9 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
+      <c r="M2" t="s">
+        <v>1847</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
@@ -6466,6 +6528,9 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
+      <c r="M3" t="s">
+        <v>1859</v>
+      </c>
       <c r="N3" s="2" t="s">
         <v>32</v>
       </c>
@@ -6516,6 +6581,9 @@
       <c r="L4" t="s">
         <v>41</v>
       </c>
+      <c r="M4" t="s">
+        <v>1848</v>
+      </c>
       <c r="N4" s="2" t="s">
         <v>42</v>
       </c>
@@ -6566,6 +6634,9 @@
       <c r="L5" t="s">
         <v>51</v>
       </c>
+      <c r="M5" t="s">
+        <v>1849</v>
+      </c>
       <c r="N5" s="2" t="s">
         <v>52</v>
       </c>
@@ -6616,6 +6687,9 @@
       <c r="L6" t="s">
         <v>60</v>
       </c>
+      <c r="M6" t="s">
+        <v>1850</v>
+      </c>
       <c r="N6" s="2" t="s">
         <v>42</v>
       </c>
@@ -6629,7 +6703,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3377852</v>
       </c>
@@ -6665,6 +6739,9 @@
       </c>
       <c r="L7" t="s">
         <v>67</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1851</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>29</v>
@@ -6716,6 +6793,9 @@
       <c r="L8" t="s">
         <v>75</v>
       </c>
+      <c r="M8" t="s">
+        <v>1852</v>
+      </c>
       <c r="N8" s="2" t="s">
         <v>52</v>
       </c>
@@ -6766,6 +6846,9 @@
       <c r="L9" t="s">
         <v>83</v>
       </c>
+      <c r="M9" t="s">
+        <v>1859</v>
+      </c>
       <c r="N9" s="2" t="s">
         <v>84</v>
       </c>
@@ -6816,6 +6899,9 @@
       <c r="L10" t="s">
         <v>93</v>
       </c>
+      <c r="M10" t="s">
+        <v>1853</v>
+      </c>
       <c r="N10" s="2" t="s">
         <v>94</v>
       </c>
@@ -6866,6 +6952,9 @@
       <c r="L11" t="s">
         <v>102</v>
       </c>
+      <c r="M11" t="s">
+        <v>1854</v>
+      </c>
       <c r="N11" s="2" t="s">
         <v>29</v>
       </c>
@@ -6916,6 +7005,9 @@
       <c r="L12" t="s">
         <v>111</v>
       </c>
+      <c r="M12" t="s">
+        <v>1855</v>
+      </c>
       <c r="N12" s="2" t="s">
         <v>112</v>
       </c>
@@ -6966,6 +7058,9 @@
       <c r="L13" t="s">
         <v>121</v>
       </c>
+      <c r="M13" t="s">
+        <v>1847</v>
+      </c>
       <c r="N13" s="2" t="s">
         <v>91</v>
       </c>
@@ -7016,6 +7111,9 @@
       <c r="L14" t="s">
         <v>130</v>
       </c>
+      <c r="M14" t="s">
+        <v>1849</v>
+      </c>
       <c r="N14" s="2" t="s">
         <v>32</v>
       </c>
@@ -7066,6 +7164,9 @@
       <c r="L15" t="s">
         <v>139</v>
       </c>
+      <c r="M15" t="s">
+        <v>1811</v>
+      </c>
       <c r="N15" s="2" t="s">
         <v>22</v>
       </c>
@@ -7116,6 +7217,9 @@
       <c r="L16" t="s">
         <v>147</v>
       </c>
+      <c r="M16" t="s">
+        <v>1849</v>
+      </c>
       <c r="N16" s="2" t="s">
         <v>32</v>
       </c>
@@ -7166,6 +7270,9 @@
       <c r="L17" t="s">
         <v>156</v>
       </c>
+      <c r="M17" t="s">
+        <v>1856</v>
+      </c>
       <c r="N17" s="2" t="s">
         <v>157</v>
       </c>
@@ -7216,6 +7323,9 @@
       <c r="L18" t="s">
         <v>165</v>
       </c>
+      <c r="M18" t="s">
+        <v>1857</v>
+      </c>
       <c r="N18" s="2" t="s">
         <v>166</v>
       </c>
@@ -7266,6 +7376,9 @@
       <c r="L19" t="s">
         <v>173</v>
       </c>
+      <c r="M19" t="s">
+        <v>1850</v>
+      </c>
       <c r="N19" s="2" t="s">
         <v>58</v>
       </c>
@@ -7316,6 +7429,9 @@
       <c r="L20" t="s">
         <v>179</v>
       </c>
+      <c r="M20" t="s">
+        <v>1811</v>
+      </c>
       <c r="N20" s="2" t="s">
         <v>29</v>
       </c>
@@ -7366,6 +7482,9 @@
       <c r="L21" t="s">
         <v>186</v>
       </c>
+      <c r="M21" t="s">
+        <v>1811</v>
+      </c>
       <c r="N21" s="2" t="s">
         <v>145</v>
       </c>
@@ -7416,6 +7535,9 @@
       <c r="L22" t="s">
         <v>195</v>
       </c>
+      <c r="M22" t="s">
+        <v>1859</v>
+      </c>
       <c r="N22" s="2" t="s">
         <v>94</v>
       </c>
@@ -7466,6 +7588,9 @@
       <c r="L23" t="s">
         <v>202</v>
       </c>
+      <c r="M23" t="s">
+        <v>1858</v>
+      </c>
       <c r="N23" s="2" t="s">
         <v>42</v>
       </c>
@@ -7516,6 +7641,9 @@
       <c r="L24" t="s">
         <v>211</v>
       </c>
+      <c r="M24" t="s">
+        <v>1849</v>
+      </c>
       <c r="N24" s="2" t="s">
         <v>212</v>
       </c>
@@ -7566,6 +7694,9 @@
       <c r="L25" t="s">
         <v>219</v>
       </c>
+      <c r="M25" t="s">
+        <v>1859</v>
+      </c>
       <c r="N25" s="2" t="s">
         <v>32</v>
       </c>
@@ -7616,6 +7747,9 @@
       <c r="L26" t="s">
         <v>226</v>
       </c>
+      <c r="M26" t="s">
+        <v>1849</v>
+      </c>
       <c r="N26" s="2" t="s">
         <v>227</v>
       </c>
@@ -7666,6 +7800,9 @@
       <c r="L27" t="s">
         <v>235</v>
       </c>
+      <c r="M27" t="s">
+        <v>1811</v>
+      </c>
       <c r="N27" s="2" t="s">
         <v>29</v>
       </c>
@@ -7716,6 +7853,9 @@
       <c r="L28" t="s">
         <v>243</v>
       </c>
+      <c r="M28" t="s">
+        <v>1854</v>
+      </c>
       <c r="N28" s="2" t="s">
         <v>29</v>
       </c>
@@ -7766,6 +7906,9 @@
       <c r="L29" t="s">
         <v>251</v>
       </c>
+      <c r="M29" t="s">
+        <v>1859</v>
+      </c>
       <c r="N29" s="2" t="s">
         <v>52</v>
       </c>
@@ -7816,6 +7959,9 @@
       <c r="L30" t="s">
         <v>259</v>
       </c>
+      <c r="M30" t="s">
+        <v>1850</v>
+      </c>
       <c r="N30" s="2" t="s">
         <v>257</v>
       </c>
@@ -7866,6 +8012,9 @@
       <c r="L31" t="s">
         <v>266</v>
       </c>
+      <c r="M31" t="s">
+        <v>1860</v>
+      </c>
       <c r="N31" s="2" t="s">
         <v>29</v>
       </c>
@@ -7916,6 +8065,9 @@
       <c r="L32" t="s">
         <v>274</v>
       </c>
+      <c r="M32" t="s">
+        <v>1849</v>
+      </c>
       <c r="N32" s="2" t="s">
         <v>94</v>
       </c>
@@ -7966,6 +8118,9 @@
       <c r="L33" t="s">
         <v>281</v>
       </c>
+      <c r="M33" t="s">
+        <v>1861</v>
+      </c>
       <c r="N33" s="2" t="s">
         <v>277</v>
       </c>
@@ -8016,6 +8171,9 @@
       <c r="L34" t="s">
         <v>289</v>
       </c>
+      <c r="M34" t="s">
+        <v>1811</v>
+      </c>
       <c r="N34" s="2" t="s">
         <v>29</v>
       </c>
@@ -8066,6 +8224,9 @@
       <c r="L35" t="s">
         <v>298</v>
       </c>
+      <c r="M35" t="s">
+        <v>1855</v>
+      </c>
       <c r="N35" s="2" t="s">
         <v>296</v>
       </c>
@@ -8116,6 +8277,9 @@
       <c r="L36" t="s">
         <v>306</v>
       </c>
+      <c r="M36" t="s">
+        <v>1851</v>
+      </c>
       <c r="N36" s="2" t="s">
         <v>52</v>
       </c>
@@ -8129,7 +8293,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="240" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="245" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3542558</v>
       </c>
@@ -8165,6 +8329,9 @@
       </c>
       <c r="L37" t="s">
         <v>315</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1862</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>310</v>
@@ -8216,6 +8383,9 @@
       <c r="L38" t="s">
         <v>323</v>
       </c>
+      <c r="M38" t="s">
+        <v>1857</v>
+      </c>
       <c r="N38" s="2" t="s">
         <v>324</v>
       </c>
@@ -8266,6 +8436,9 @@
       <c r="L39" t="s">
         <v>332</v>
       </c>
+      <c r="M39" t="s">
+        <v>1849</v>
+      </c>
       <c r="N39" s="2" t="s">
         <v>145</v>
       </c>
@@ -8316,6 +8489,9 @@
       <c r="L40" t="s">
         <v>339</v>
       </c>
+      <c r="M40" t="s">
+        <v>1811</v>
+      </c>
       <c r="N40" s="2" t="s">
         <v>145</v>
       </c>
@@ -8366,6 +8542,9 @@
       <c r="L41" t="s">
         <v>347</v>
       </c>
+      <c r="M41" t="s">
+        <v>1811</v>
+      </c>
       <c r="N41" s="2" t="s">
         <v>29</v>
       </c>
@@ -8416,6 +8595,9 @@
       <c r="L42" t="s">
         <v>355</v>
       </c>
+      <c r="M42" t="s">
+        <v>1811</v>
+      </c>
       <c r="N42" s="2" t="s">
         <v>356</v>
       </c>
@@ -8466,6 +8648,9 @@
       <c r="L43" t="s">
         <v>363</v>
       </c>
+      <c r="M43" t="s">
+        <v>1865</v>
+      </c>
       <c r="N43" s="2" t="s">
         <v>212</v>
       </c>
@@ -8516,6 +8701,9 @@
       <c r="L44" t="s">
         <v>371</v>
       </c>
+      <c r="M44" t="s">
+        <v>1811</v>
+      </c>
       <c r="N44" s="2" t="s">
         <v>372</v>
       </c>
@@ -8566,6 +8754,9 @@
       <c r="L45" t="s">
         <v>378</v>
       </c>
+      <c r="M45" t="s">
+        <v>1850</v>
+      </c>
       <c r="N45" s="2" t="s">
         <v>212</v>
       </c>
@@ -8616,6 +8807,9 @@
       <c r="L46" t="s">
         <v>386</v>
       </c>
+      <c r="M46" t="s">
+        <v>1850</v>
+      </c>
       <c r="N46" s="2" t="s">
         <v>145</v>
       </c>
@@ -8666,6 +8860,9 @@
       <c r="L47" t="s">
         <v>393</v>
       </c>
+      <c r="M47" t="s">
+        <v>1865</v>
+      </c>
       <c r="N47" s="2" t="s">
         <v>394</v>
       </c>
@@ -8716,6 +8913,9 @@
       <c r="L48" t="s">
         <v>403</v>
       </c>
+      <c r="M48" t="s">
+        <v>1864</v>
+      </c>
       <c r="N48" s="2" t="s">
         <v>145</v>
       </c>
@@ -8766,6 +8966,9 @@
       <c r="L49" t="s">
         <v>412</v>
       </c>
+      <c r="M49" t="s">
+        <v>1850</v>
+      </c>
       <c r="N49" s="2" t="s">
         <v>413</v>
       </c>
@@ -8816,6 +9019,9 @@
       <c r="L50" t="s">
         <v>421</v>
       </c>
+      <c r="M50" t="s">
+        <v>1851</v>
+      </c>
       <c r="N50" s="2" t="s">
         <v>52</v>
       </c>
@@ -8866,6 +9072,9 @@
       <c r="L51" t="s">
         <v>429</v>
       </c>
+      <c r="M51" t="s">
+        <v>1864</v>
+      </c>
       <c r="N51" s="2" t="s">
         <v>84</v>
       </c>
@@ -8916,6 +9125,9 @@
       <c r="L52" t="s">
         <v>437</v>
       </c>
+      <c r="M52" t="s">
+        <v>1865</v>
+      </c>
       <c r="N52" s="2" t="s">
         <v>145</v>
       </c>
@@ -8966,6 +9178,9 @@
       <c r="L53" t="s">
         <v>444</v>
       </c>
+      <c r="M53" t="s">
+        <v>1859</v>
+      </c>
       <c r="N53" s="2" t="s">
         <v>52</v>
       </c>
@@ -9016,6 +9231,9 @@
       <c r="L54" t="s">
         <v>452</v>
       </c>
+      <c r="M54" t="s">
+        <v>1849</v>
+      </c>
       <c r="N54" s="2" t="s">
         <v>84</v>
       </c>
@@ -9066,6 +9284,9 @@
       <c r="L55" t="s">
         <v>460</v>
       </c>
+      <c r="M55" t="s">
+        <v>1811</v>
+      </c>
       <c r="N55" s="2" t="s">
         <v>461</v>
       </c>
@@ -9116,6 +9337,9 @@
       <c r="L56" t="s">
         <v>468</v>
       </c>
+      <c r="M56" t="s">
+        <v>1857</v>
+      </c>
       <c r="N56" s="2" t="s">
         <v>145</v>
       </c>
@@ -9166,6 +9390,9 @@
       <c r="L57" t="s">
         <v>475</v>
       </c>
+      <c r="M57" t="s">
+        <v>1866</v>
+      </c>
       <c r="N57" s="2" t="s">
         <v>476</v>
       </c>
@@ -9216,6 +9443,9 @@
       <c r="L58" t="s">
         <v>483</v>
       </c>
+      <c r="M58" t="s">
+        <v>1811</v>
+      </c>
       <c r="N58" s="2" t="s">
         <v>479</v>
       </c>
@@ -9266,6 +9496,9 @@
       <c r="L59" t="s">
         <v>490</v>
       </c>
+      <c r="M59" t="s">
+        <v>1852</v>
+      </c>
       <c r="N59" s="2" t="s">
         <v>491</v>
       </c>
@@ -9316,6 +9549,9 @@
       <c r="L60" t="s">
         <v>499</v>
       </c>
+      <c r="M60" t="s">
+        <v>1859</v>
+      </c>
       <c r="N60" s="2" t="s">
         <v>84</v>
       </c>
@@ -9366,6 +9602,9 @@
       <c r="L61" t="s">
         <v>507</v>
       </c>
+      <c r="M61" t="s">
+        <v>1866</v>
+      </c>
       <c r="N61" s="2" t="s">
         <v>508</v>
       </c>
@@ -9416,6 +9655,9 @@
       <c r="L62" t="s">
         <v>515</v>
       </c>
+      <c r="M62" t="s">
+        <v>1811</v>
+      </c>
       <c r="N62" s="2" t="s">
         <v>145</v>
       </c>
@@ -9466,6 +9708,9 @@
       <c r="L63" t="s">
         <v>522</v>
       </c>
+      <c r="M63" t="s">
+        <v>1849</v>
+      </c>
       <c r="N63" s="2" t="s">
         <v>523</v>
       </c>
@@ -9516,6 +9761,9 @@
       <c r="L64" t="s">
         <v>530</v>
       </c>
+      <c r="M64" t="s">
+        <v>1854</v>
+      </c>
       <c r="N64" s="2" t="s">
         <v>531</v>
       </c>
@@ -9566,6 +9814,9 @@
       <c r="L65" t="s">
         <v>538</v>
       </c>
+      <c r="M65" t="s">
+        <v>1852</v>
+      </c>
       <c r="N65" s="2" t="s">
         <v>491</v>
       </c>
@@ -9616,6 +9867,9 @@
       <c r="L66" t="s">
         <v>545</v>
       </c>
+      <c r="M66" t="s">
+        <v>1856</v>
+      </c>
       <c r="N66" s="2" t="s">
         <v>541</v>
       </c>
@@ -9666,6 +9920,9 @@
       <c r="L67" t="s">
         <v>552</v>
       </c>
+      <c r="M67" t="s">
+        <v>1855</v>
+      </c>
       <c r="N67" s="2" t="s">
         <v>29</v>
       </c>
@@ -9716,6 +9973,9 @@
       <c r="L68" t="s">
         <v>559</v>
       </c>
+      <c r="M68" t="s">
+        <v>1811</v>
+      </c>
       <c r="N68" s="2" t="s">
         <v>29</v>
       </c>
@@ -9766,6 +10026,9 @@
       <c r="L69" t="s">
         <v>567</v>
       </c>
+      <c r="M69" t="s">
+        <v>1811</v>
+      </c>
       <c r="N69" s="2" t="s">
         <v>145</v>
       </c>
@@ -9816,6 +10079,9 @@
       <c r="L70" t="s">
         <v>575</v>
       </c>
+      <c r="M70" t="s">
+        <v>1811</v>
+      </c>
       <c r="N70" s="2" t="s">
         <v>573</v>
       </c>
@@ -9866,6 +10132,9 @@
       <c r="L71" t="s">
         <v>583</v>
       </c>
+      <c r="M71" t="s">
+        <v>1850</v>
+      </c>
       <c r="N71" s="2" t="s">
         <v>579</v>
       </c>
@@ -9916,6 +10185,9 @@
       <c r="L72" t="s">
         <v>590</v>
       </c>
+      <c r="M72" t="s">
+        <v>1849</v>
+      </c>
       <c r="N72" s="2" t="s">
         <v>29</v>
       </c>
@@ -9966,6 +10238,9 @@
       <c r="L73" t="s">
         <v>597</v>
       </c>
+      <c r="M73" t="s">
+        <v>1811</v>
+      </c>
       <c r="N73" s="2" t="s">
         <v>145</v>
       </c>
@@ -10016,6 +10291,9 @@
       <c r="L74" t="s">
         <v>604</v>
       </c>
+      <c r="M74" t="s">
+        <v>1811</v>
+      </c>
       <c r="N74" s="2" t="s">
         <v>605</v>
       </c>
@@ -10066,6 +10344,9 @@
       <c r="L75" t="s">
         <v>612</v>
       </c>
+      <c r="M75" t="s">
+        <v>1811</v>
+      </c>
       <c r="N75" s="2" t="s">
         <v>29</v>
       </c>
@@ -10116,6 +10397,9 @@
       <c r="L76" t="s">
         <v>619</v>
       </c>
+      <c r="M76" t="s">
+        <v>1857</v>
+      </c>
       <c r="N76" s="2" t="s">
         <v>615</v>
       </c>
@@ -10166,6 +10450,9 @@
       <c r="L77" t="s">
         <v>627</v>
       </c>
+      <c r="M77" t="s">
+        <v>1850</v>
+      </c>
       <c r="N77" s="2" t="s">
         <v>145</v>
       </c>
@@ -10216,6 +10503,9 @@
       <c r="L78" t="s">
         <v>634</v>
       </c>
+      <c r="M78" t="s">
+        <v>1852</v>
+      </c>
       <c r="N78" s="2" t="s">
         <v>32</v>
       </c>
@@ -10266,6 +10556,9 @@
       <c r="L79" t="s">
         <v>641</v>
       </c>
+      <c r="M79" t="s">
+        <v>1863</v>
+      </c>
       <c r="N79" s="2" t="s">
         <v>84</v>
       </c>
@@ -10316,6 +10609,9 @@
       <c r="L80" t="s">
         <v>648</v>
       </c>
+      <c r="M80" t="s">
+        <v>1811</v>
+      </c>
       <c r="N80" s="2" t="s">
         <v>29</v>
       </c>
@@ -10366,6 +10662,9 @@
       <c r="L81" t="s">
         <v>656</v>
       </c>
+      <c r="M81" t="s">
+        <v>1864</v>
+      </c>
       <c r="N81" s="2" t="s">
         <v>29</v>
       </c>
@@ -10416,6 +10715,9 @@
       <c r="L82" t="s">
         <v>663</v>
       </c>
+      <c r="M82" t="s">
+        <v>1854</v>
+      </c>
       <c r="N82" s="2" t="s">
         <v>664</v>
       </c>
@@ -10466,6 +10768,9 @@
       <c r="L83" t="s">
         <v>672</v>
       </c>
+      <c r="M83" t="s">
+        <v>1811</v>
+      </c>
       <c r="N83" s="2" t="s">
         <v>145</v>
       </c>
@@ -10516,6 +10821,9 @@
       <c r="L84" t="s">
         <v>679</v>
       </c>
+      <c r="M84" t="s">
+        <v>1849</v>
+      </c>
       <c r="N84" s="2" t="s">
         <v>680</v>
       </c>
@@ -10566,6 +10874,9 @@
       <c r="L85" t="s">
         <v>686</v>
       </c>
+      <c r="M85" t="s">
+        <v>1856</v>
+      </c>
       <c r="N85" s="2" t="s">
         <v>687</v>
       </c>
@@ -10616,6 +10927,9 @@
       <c r="L86" t="s">
         <v>695</v>
       </c>
+      <c r="M86" t="s">
+        <v>1850</v>
+      </c>
       <c r="N86" s="2" t="s">
         <v>696</v>
       </c>
@@ -10666,6 +10980,9 @@
       <c r="L87" t="s">
         <v>703</v>
       </c>
+      <c r="M87" t="s">
+        <v>1811</v>
+      </c>
       <c r="N87" s="2" t="s">
         <v>29</v>
       </c>
@@ -10716,6 +11033,9 @@
       <c r="L88" t="s">
         <v>710</v>
       </c>
+      <c r="M88" t="s">
+        <v>1853</v>
+      </c>
       <c r="N88" s="2" t="s">
         <v>711</v>
       </c>
@@ -10765,6 +11085,9 @@
       </c>
       <c r="L89" t="s">
         <v>718</v>
+      </c>
+      <c r="M89" t="s">
+        <v>1849</v>
       </c>
       <c r="N89" s="2" t="s">
         <v>145</v>

</xml_diff>